<commit_message>
Added investor kyc import test
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8E1DA6-3600-47E4-A2FF-196A30456A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56598754-44FE-4E3D-975A-21E1E51FBA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>IFSC Code</t>
   </si>
   <si>
-    <t>Arun Gupta</t>
-  </si>
-  <si>
     <t>AGUPC8572B</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>HDFC0001755</t>
   </si>
   <si>
-    <t>Sekhsaria family office</t>
-  </si>
-  <si>
     <t>Send Confirmation Email</t>
   </si>
   <si>
@@ -98,6 +92,12 @@
   </si>
   <si>
     <t>Two</t>
+  </si>
+  <si>
+    <t>Investor 1</t>
+  </si>
+  <si>
+    <t>Investor 2</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -505,71 +505,71 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
       <c r="H2">
         <v>50100033849984</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
       <c r="H3">
         <v>50100033849985</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added phone to investor_kyc import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56598754-44FE-4E3D-975A-21E1E51FBA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A75489-8E57-4940-9486-DA49E972515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Investor</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Investor 2</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -470,13 +473,14 @@
     <col min="3" max="3" width="14.3125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.8125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.8125" customWidth="1"/>
+    <col min="7" max="7" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,22 +497,25 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -524,23 +531,26 @@
       <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1">
+        <v>999999999</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>50100033849984</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -556,19 +566,22 @@
       <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1">
+        <v>111111111</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>50100033849985</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed user from investor kyc
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE6A9CA-E1E1-4227-9D9F-54D7EFD8D245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3DF0C-C34C-4EB4-8974-13E60D0B6B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Investor</t>
   </si>
@@ -28,12 +28,6 @@
     <t>Full Name</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>PAN</t>
   </si>
   <si>
@@ -55,68 +49,37 @@
     <t>HDFC0001755</t>
   </si>
   <si>
-    <t>Send Confirmation Email</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Import</t>
-  </si>
-  <si>
     <t>Import 1</t>
   </si>
   <si>
     <t>Import 2</t>
   </si>
   <si>
-    <t>import1@ag.com</t>
-  </si>
-  <si>
-    <t>import2@sfo.com</t>
-  </si>
-  <si>
     <t>AGUPC8572C</t>
   </si>
   <si>
     <t>D110</t>
   </si>
   <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>Two</t>
-  </si>
-  <si>
     <t>Investor 1</t>
   </si>
   <si>
     <t>Investor 2</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
+    <t>Verified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="1"/>
     </font>
@@ -138,16 +101,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -471,16 +431,12 @@
     <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.8125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.8125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.8125" customWidth="1"/>
-    <col min="7" max="7" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,102 +450,62 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="E2">
+        <v>50100033849984</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1">
-        <v>999999999</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>50100033849985</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G3" t="s">
         <v>9</v>
-      </c>
-      <c r="I2">
-        <v>50100033849984</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1">
-        <v>111111111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>50100033849985</v>
-      </c>
-      <c r="J3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{A3BFD3CB-1CBC-4131-A74E-40486B56B63B}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{093E4352-CBAE-41E3-87BC-9C22BC1B155E}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added residency to kyc import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B5FB8D-1AB2-4587-87C1-2434DB1A5A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2FA8C7-CA4C-4A00-99F0-B3ECA526A8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Investor</t>
   </si>
@@ -87,9 +87,6 @@
     <t>D110</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Individual</t>
   </si>
   <si>
@@ -106,6 +103,18 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>KYC Type</t>
+  </si>
+  <si>
+    <t>Residency</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>Foreign</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -470,13 +479,13 @@
     <col min="1" max="1" width="28.625" customWidth="1"/>
     <col min="2" max="2" width="19.8125" customWidth="1"/>
     <col min="3" max="3" width="14.3125" customWidth="1"/>
-    <col min="4" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="18.6875" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="4" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="18.6875" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,31 +499,34 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -528,28 +540,31 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
         <v>50100033849984</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
-        <v>25</v>
+      <c r="L2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -563,25 +578,28 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
         <v>50100033849985</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
-        <v>26</v>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed kyc import cols
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90C628E-706F-45F3-9084-52BA362E2C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2F42E2-CA3A-42EA-B3DF-85885B4F2B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Investor</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Bank Account</t>
-  </si>
-  <si>
     <t>IFSC Code</t>
   </si>
   <si>
@@ -109,6 +106,42 @@
   </si>
   <si>
     <t>Investor 4</t>
+  </si>
+  <si>
+    <t>Correspondence Address</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>BOB</t>
+  </si>
+  <si>
+    <t>HDFC</t>
+  </si>
+  <si>
+    <t>Xyz</t>
+  </si>
+  <si>
+    <t>Abc</t>
   </si>
 </sst>
 </file>
@@ -143,11 +176,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,24 +496,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.625" customWidth="1"/>
     <col min="2" max="2" width="19.8125" customWidth="1"/>
-    <col min="3" max="3" width="14.3125" customWidth="1"/>
-    <col min="4" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="18.6875" customWidth="1"/>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.5625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3125" customWidth="1"/>
+    <col min="5" max="10" width="11" customWidth="1"/>
+    <col min="11" max="12" width="18.6875" customWidth="1"/>
+    <col min="13" max="13" width="15.375" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,117 +522,156 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>27478</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2">
+        <v>50100033849984</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15772</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3">
+        <v>50100033849985</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2">
-        <v>50100033849984</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="N3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
+      <c r="P3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="G3">
-        <v>50100033849985</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="P4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
+      <c r="P5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for auto creation of FCF from KYCs
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2F42E2-CA3A-42EA-B3DF-85885B4F2B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FD883E-30E6-4A00-8934-AA6312D10905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Investor</t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t>Abc</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Sir</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -496,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +529,7 @@
     <col min="16" max="16" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +578,14 @@
       <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -610,8 +631,14 @@
       <c r="P2" t="s">
         <v>13</v>
       </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -657,8 +684,14 @@
       <c r="P3" t="s">
         <v>13</v>
       </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -666,7 +699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added instrument to cashflows (#204)
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Desktop\bulk files with notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C2F037-D735-4BFA-9A98-AA9974D05F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEF86A9-1AED-42B4-93A7-D608E7CF6F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InvestorKyc" sheetId="1" r:id="rId1"/>
@@ -1083,7 +1083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="80" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1207,7 +1209,7 @@
         <v>4</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>41</v>
@@ -1258,7 +1260,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added agrement unit type to investor kyc upload (#269)
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -484,12 +484,37 @@
             <family val="0"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">-Mandatory for Angel Funds
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Arial"/>
+            <family val="1"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">-Mandatory
 -As per SEBI reporting requirements</t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -514,7 +539,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +579,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t xml:space="preserve">Investor</t>
   </si>
@@ -610,6 +635,9 @@
     <t xml:space="preserve">Agreement Committed Amount</t>
   </si>
   <si>
+    <t xml:space="preserve">Agreement Unit Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sebi Investor Category</t>
   </si>
   <si>
@@ -661,6 +689,9 @@
     <t xml:space="preserve">signatory1@gmail.com,signatory2@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
@@ -688,6 +719,9 @@
     <t xml:space="preserve">BOB0001</t>
   </si>
   <si>
+    <t xml:space="preserve">A2</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
@@ -721,6 +755,9 @@
     <t xml:space="preserve">signatory2@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">A3</t>
+  </si>
+  <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
@@ -743,6 +780,9 @@
   </si>
   <si>
     <t xml:space="preserve">Axis0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -981,13 +1021,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.06"/>
@@ -1006,14 +1046,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="11.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="22" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="11.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="1" width="8.62"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1079,244 +1118,259 @@
       </c>
       <c r="V1" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>27478</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>50100000000</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R2" s="6" t="n">
         <v>1000000</v>
       </c>
-      <c r="S2" s="6"/>
+      <c r="S2" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="T2" s="6"/>
-      <c r="U2" s="1" t="n">
+      <c r="U2" s="6"/>
+      <c r="V2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>35</v>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>15772</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>50100000001</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R3" s="1" t="n">
         <v>2000000</v>
       </c>
-      <c r="U3" s="1" t="n">
+      <c r="S3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>44</v>
+      <c r="W3" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>33529</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>50100000002</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>3000000</v>
       </c>
-      <c r="U4" s="1" t="n">
+      <c r="S4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>55</v>
+      <c r="W4" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>36676</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>50100000003</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="R5" s="1" t="n">
         <v>4000000</v>
       </c>
-      <c r="U5" s="1" t="n">
+      <c r="S5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>63</v>
+      <c r="W5" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added suppor for kyc update where name or pan is nil
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CDE01E-E10E-4204-A127-AA88F421FEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED4A9DD-B9CA-4D4A-856D-24F0F698803C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,7 +565,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>Investor</t>
   </si>
@@ -748,9 +748,6 @@
   </si>
   <si>
     <t>Investor 4</t>
-  </si>
-  <si>
-    <t>Import 4</t>
   </si>
   <si>
     <t>AGUPC8572F</t>
@@ -1254,7 +1251,7 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -1545,17 +1542,14 @@
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="C5" s="4">
         <v>36676</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>52</v>
@@ -1564,10 +1558,10 @@
         <v>42</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="K5" s="1">
         <v>50100000003</v>
@@ -1576,7 +1570,7 @@
         <v>55</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>34</v>
@@ -1594,13 +1588,13 @@
         <v>4000000</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V5" s="1">
         <v>4</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added better check in ImportUtil to update the form_type, only for nil form_type_id
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t xml:space="preserve">Investor</t>
   </si>
@@ -574,6 +574,9 @@
     <t xml:space="preserve">Custom field   2</t>
   </si>
   <si>
+    <t xml:space="preserve">Form Tag</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investor 1</t>
   </si>
   <si>
@@ -616,6 +619,9 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investor 2</t>
   </si>
   <si>
@@ -644,6 +650,9 @@
   </si>
   <si>
     <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gift City</t>
   </si>
   <si>
     <t xml:space="preserve">Investor 3</t>
@@ -831,32 +840,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1110,16 +1123,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.5"/>
@@ -1128,317 +1141,326 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="11.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="11.92"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="21" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="2" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="n">
         <v>27478</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>50100000000</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="6" t="n">
+      <c r="Q2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="7" t="n">
         <v>1000000</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>33</v>
+      <c r="S2" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="T2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="C3" s="5" t="n">
         <v>15772</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>50100000001</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="R3" s="1" t="n">
         <v>2000000</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="T3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="n">
         <v>33529</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>50100000002</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>3000000</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="T4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="4" t="n">
+        <v>58</v>
+      </c>
+      <c r="C5" s="5" t="n">
         <v>36676</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>50100000003</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R5" s="1" t="n">
         <v>4000000</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="T5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>